<commit_message>
Working Invoice Sorting. Supports failed invoice and an auto email reply for the receipt.
</commit_message>
<xml_diff>
--- a/InvoiceScannerSrc/customer_emails.xlsx
+++ b/InvoiceScannerSrc/customer_emails.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Derek\raffettosBlueSystemAddons\InvoiceScannerSrc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{437C7663-2AC8-40DB-9BC6-C7BFD33A7DD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CEFC894-AA07-421F-B0B7-BD642C0BBCB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
     <t>garret@gmail.com</t>
   </si>
   <si>
-    <t>customerid</t>
+    <t>BUONAN</t>
   </si>
 </sst>
 </file>
@@ -368,7 +368,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated duplicate invoice creation. Also updated unsorted invoice deletion from original invoices folder
</commit_message>
<xml_diff>
--- a/InvoiceScannerSrc/customer_emails.xlsx
+++ b/InvoiceScannerSrc/customer_emails.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Derek\raffettosBlueSystemAddons\InvoiceScannerSrc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raffetto\Desktop\DerekRaffettoCode\raffettosBlueSystemAddons\InvoiceScannerSrc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CEFC894-AA07-421F-B0B7-BD642C0BBCB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6B0DD8B-6F72-43E5-AC36-4E7216A254D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="16740" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -365,10 +365,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -389,6 +389,9 @@
         <v>2</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3" s="1"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B1" r:id="rId1" xr:uid="{A8D74881-0BB6-464E-BC41-415D3E50D2CC}"/>

</xml_diff>

<commit_message>
Added combinations for product codes, fixed last row issue, and made sure qty shipped gets read from the document
</commit_message>
<xml_diff>
--- a/InvoiceScannerSrc/customer_emails.xlsx
+++ b/InvoiceScannerSrc/customer_emails.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raffetto\Desktop\DerekRaffettoCode\raffettosBlueSystemAddons\InvoiceScannerSrc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6B0DD8B-6F72-43E5-AC36-4E7216A254D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95BD23F4-EEFB-4E26-8AFD-3B86201EF65D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="16740" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>gingoso2@gmail.com</t>
   </si>
@@ -37,6 +37,9 @@
   </si>
   <si>
     <t>BUONAN</t>
+  </si>
+  <si>
+    <t>JENNYS</t>
   </si>
 </sst>
 </file>
@@ -368,7 +371,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -390,12 +393,18 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B3" s="1"/>
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B1" r:id="rId1" xr:uid="{A8D74881-0BB6-464E-BC41-415D3E50D2CC}"/>
     <hyperlink ref="B2" r:id="rId2" xr:uid="{33BD8C6B-EF33-4672-9860-80BE4BD21E94}"/>
+    <hyperlink ref="B3" r:id="rId3" xr:uid="{2CE7CAE3-1EDB-4CE2-A498-974193D950A5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>